<commit_message>
Todo bien puesto ahora
</commit_message>
<xml_diff>
--- a/The Hampered Traveling Postman Problem with Segments/table_results.xlsx
+++ b/The Hampered Traveling Postman Problem with Segments/table_results.xlsx
@@ -2172,8 +2172,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CC872E1270CB784E9B98D50896A839F6" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6e94c8e1f570b253bc5c1b36e6421b98">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="116ddbad-b67c-4622-b846-55da43670eb8" xmlns:ns3="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="560abf7957fee032e721452e984d1162" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CC872E1270CB784E9B98D50896A839F6" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="d843d1c7e7f025820150451ac71dab0b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="116ddbad-b67c-4622-b846-55da43670eb8" xmlns:ns3="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d7d841d9c1cdff30d97ae0bcf8819b27" ns2:_="" ns3:_="">
     <xsd:import namespace="116ddbad-b67c-4622-b846-55da43670eb8"/>
     <xsd:import namespace="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe"/>
     <xsd:element name="properties">
@@ -2195,6 +2195,7 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2260,6 +2261,11 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="0838a0db-6cb4-4fef-a3f8-577e3ea6a4fe" elementFormDefault="qualified">
@@ -2420,5 +2426,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C6FC1E1-67C8-4403-B013-431AAF32A17C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96DBAE8A-F78B-47FE-8105-1445B1BB9560}"/>
 </file>
</xml_diff>